<commit_message>
Initial commit on new update
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F726F59-E42D-46D5-AD07-409FA9923B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605680D5-17E9-45DB-B59A-97E637870A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="108">
   <si>
     <t>indicatorCategory</t>
   </si>
@@ -214,9 +214,6 @@
     <t>(Y/N)</t>
   </si>
   <si>
-    <t>Chicken Eggs Sold</t>
-  </si>
-  <si>
     <t>Chicken Headcount Net Change</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>Sale Price</t>
   </si>
   <si>
-    <t>Eggs Sold</t>
-  </si>
-  <si>
     <t>Eggs Per Day</t>
   </si>
   <si>
@@ -338,6 +332,18 @@
   </si>
   <si>
     <t>Price of last sale</t>
+  </si>
+  <si>
+    <t>Eggs Sold (Y/N)</t>
+  </si>
+  <si>
+    <t>Eggs Sold (Qty)</t>
+  </si>
+  <si>
+    <t>Household Sold Eggs</t>
+  </si>
+  <si>
+    <t>Number of Chicken Eggs Sold</t>
   </si>
 </sst>
 </file>
@@ -698,7 +704,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,13 +728,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
@@ -757,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -789,7 +795,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
@@ -810,7 +816,7 @@
         <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -821,7 +827,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -842,7 +848,7 @@
         <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -853,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -885,13 +891,13 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
         <v>46</v>
@@ -906,7 +912,7 @@
         <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -917,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
@@ -938,7 +944,7 @@
         <v>35</v>
       </c>
       <c r="K7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -949,7 +955,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
         <v>53</v>
@@ -970,7 +976,7 @@
         <v>36</v>
       </c>
       <c r="K8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -981,10 +987,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
         <v>59</v>
@@ -1013,7 +1019,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
         <v>61</v>
@@ -1034,7 +1040,7 @@
         <v>38</v>
       </c>
       <c r="K10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1045,10 +1051,10 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
         <v>63</v>
@@ -1066,7 +1072,7 @@
         <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1077,13 +1083,13 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
         <v>65</v>
-      </c>
-      <c r="E12" t="s">
-        <v>66</v>
       </c>
       <c r="F12" t="s">
         <v>46</v>
@@ -1109,13 +1115,13 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
         <v>46</v>
@@ -1130,7 +1136,7 @@
         <v>37</v>
       </c>
       <c r="K13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1141,13 +1147,13 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" t="s">
         <v>46</v>
@@ -1159,7 +1165,7 @@
         <v>25</v>
       </c>
       <c r="K14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1170,10 +1176,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
         <v>62</v>
@@ -1191,7 +1197,7 @@
         <v>38</v>
       </c>
       <c r="K15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1202,13 +1208,13 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" t="s">
         <v>46</v>
@@ -1220,7 +1226,7 @@
         <v>28</v>
       </c>
       <c r="K16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1231,13 +1237,13 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
         <v>46</v>
@@ -1249,7 +1255,7 @@
         <v>29</v>
       </c>
       <c r="K17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes and update to logic model.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EFE42B-8C32-47E7-9E03-00C34CF20E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AECBE4-57C3-487A-B697-455604DB1F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10035" yWindow="960" windowWidth="15660" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="162">
   <si>
     <t>indicatorCategory</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t xml:space="preserve">currency </t>
+  </si>
+  <si>
+    <t>poultry_livestock</t>
   </si>
 </sst>
 </file>
@@ -872,10 +875,10 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G50" sqref="G50"/>
+      <selection pane="bottomRight" activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +939,7 @@
         <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -965,7 +968,7 @@
         <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -994,7 +997,7 @@
         <v>115</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1023,7 +1026,7 @@
         <v>114</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1052,7 +1055,7 @@
         <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1081,7 +1084,7 @@
         <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1110,7 +1113,7 @@
         <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1139,7 +1142,7 @@
         <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1168,7 +1171,7 @@
         <v>119</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1197,7 +1200,7 @@
         <v>120</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1226,7 +1229,7 @@
         <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1255,7 +1258,7 @@
         <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1284,7 +1287,7 @@
         <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1310,7 +1313,7 @@
         <v>121</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1339,7 +1342,7 @@
         <v>122</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1365,7 +1368,7 @@
         <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1391,7 +1394,7 @@
         <v>124</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1414,7 +1417,7 @@
         <v>125</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1437,7 +1440,7 @@
         <v>126</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1460,7 +1463,7 @@
         <v>127</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1483,7 +1486,7 @@
         <v>128</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1506,7 +1509,7 @@
         <v>129</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1529,7 +1532,7 @@
         <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1552,7 +1555,7 @@
         <v>131</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1575,7 +1578,7 @@
         <v>132</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1598,7 +1601,7 @@
         <v>133</v>
       </c>
       <c r="E27" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1621,7 +1624,7 @@
         <v>134</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1644,7 +1647,7 @@
         <v>135</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1667,7 +1670,7 @@
         <v>157</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1690,7 +1693,7 @@
         <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1713,7 +1716,7 @@
         <v>137</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1736,7 +1739,7 @@
         <v>138</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1759,7 +1762,7 @@
         <v>130</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1782,7 +1785,7 @@
         <v>131</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1805,7 +1808,7 @@
         <v>139</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1828,7 +1831,7 @@
         <v>140</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1851,7 +1854,7 @@
         <v>141</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1874,7 +1877,7 @@
         <v>142</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -1894,7 +1897,7 @@
         <v>143</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1917,7 +1920,7 @@
         <v>144</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1940,7 +1943,7 @@
         <v>145</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1963,7 +1966,7 @@
         <v>146</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -1986,7 +1989,7 @@
         <v>147</v>
       </c>
       <c r="E44" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -2009,7 +2012,7 @@
         <v>148</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2032,7 +2035,7 @@
         <v>149</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2055,7 +2058,7 @@
         <v>151</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -2078,7 +2081,7 @@
         <v>150</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -2101,7 +2104,7 @@
         <v>152</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="F49">
         <v>1</v>

</xml_diff>

<commit_message>
Prepping for modularizing the dataset, addition of some files for transition and upating.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89EF88C-5405-4427-B3D4-B90510B1E08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B14DC7-289C-4A28-94FB-8C10E85BFCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3255" windowWidth="23355" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="2760" windowWidth="23355" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="243">
   <si>
     <t>indicatorCategory</t>
   </si>
@@ -249,9 +249,6 @@
     <t>mortality_rt_chickens</t>
   </si>
   <si>
-    <t>net_growth_pct_Chickens</t>
-  </si>
-  <si>
     <t>bought_received_Chickens</t>
   </si>
   <si>
@@ -345,9 +342,6 @@
     <t>Chicken Vaccination Rate</t>
   </si>
   <si>
-    <t>Flock Growth Rate</t>
-  </si>
-  <si>
     <t>Chickens Purchased or Received</t>
   </si>
   <si>
@@ -522,9 +516,6 @@
     <t>Live Sale Revenue (Chicken)</t>
   </si>
   <si>
-    <t xml:space="preserve">Net Growth Rate </t>
-  </si>
-  <si>
     <t>Chicken Vaccination Cost (KHR)</t>
   </si>
   <si>
@@ -561,12 +552,6 @@
     <t>Cattle Born</t>
   </si>
   <si>
-    <t>Cattle Used for Draugh (Y/N)</t>
-  </si>
-  <si>
-    <t>Cattle Used for Draught (Y/N)</t>
-  </si>
-  <si>
     <t>Daily Egg Production</t>
   </si>
   <si>
@@ -708,9 +693,6 @@
     <t>Determined by dividing "Chickens vaccinated" by "chickens owned (total)"</t>
   </si>
   <si>
-    <t>Determined by dividing "Flock Growth" by "Chickens Owned (Start)"</t>
-  </si>
-  <si>
     <t>How many chickens births did the holding have?</t>
   </si>
   <si>
@@ -829,16 +811,51 @@
   </si>
   <si>
     <t>vax_pct_Chickens</t>
+  </si>
+  <si>
+    <t>Flock Net Growth (Head)</t>
+  </si>
+  <si>
+    <t>Flock Net Growth</t>
+  </si>
+  <si>
+    <t>Fix</t>
+  </si>
+  <si>
+    <t>provision_feed_Chickens</t>
+  </si>
+  <si>
+    <t>Cattle Used for Draughting (Y/N)</t>
+  </si>
+  <si>
+    <t>Use of Chicken Feed</t>
+  </si>
+  <si>
+    <t>Percent of Households Providing Chicken Feed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1040,53 +1057,55 @@
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Enabling condition" xfId="9" xr:uid="{16A541CE-23F2-4717-B94D-AC194AA37789}"/>
@@ -1457,13 +1476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,7 +1509,7 @@
         <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -1505,10 +1524,10 @@
         <v>20</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K1" t="s">
         <v>35</v>
@@ -1522,13 +1541,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1540,10 +1559,10 @@
         <v>25</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1551,16 +1570,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -1576,7 +1595,7 @@
         <v>36</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="L3" s="4"/>
     </row>
@@ -1585,16 +1604,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
@@ -1610,7 +1629,7 @@
         <v>36</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="L4" s="4"/>
     </row>
@@ -1622,13 +1641,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1640,10 +1659,10 @@
         <v>26</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1654,13 +1673,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1672,10 +1691,10 @@
         <v>27</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1686,13 +1705,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1704,10 +1723,10 @@
         <v>28</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1718,13 +1737,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1736,10 +1755,10 @@
         <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1753,10 +1772,10 @@
         <v>37</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E9" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1768,10 +1787,10 @@
         <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1785,10 +1804,10 @@
         <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E10" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1800,10 +1819,10 @@
         <v>31</v>
       </c>
       <c r="J10" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1814,13 +1833,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1832,10 +1851,10 @@
         <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1846,13 +1865,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E12" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1864,10 +1883,10 @@
         <v>33</v>
       </c>
       <c r="J12" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1881,10 +1900,10 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1896,7 +1915,7 @@
         <v>34</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1913,7 +1932,7 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1928,7 +1947,7 @@
         <v>36</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1936,16 +1955,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1960,7 +1979,7 @@
         <v>36</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1977,7 +1996,7 @@
         <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1992,7 +2011,7 @@
         <v>36</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2006,10 +2025,10 @@
         <v>43</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2024,7 +2043,7 @@
         <v>36</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2035,13 +2054,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -2056,7 +2075,7 @@
         <v>36</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2064,16 +2083,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="E19" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2088,7 +2107,7 @@
         <v>36</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2099,22 +2118,22 @@
         <v>47</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I20" t="s">
         <v>36</v>
@@ -2123,7 +2142,7 @@
         <v>36</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2131,25 +2150,25 @@
         <v>1</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>36</v>
@@ -2158,42 +2177,40 @@
         <v>36</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>48</v>
+      <c r="B22" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>80</v>
+        <v>237</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>139</v>
+        <v>236</v>
       </c>
       <c r="E22" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>98</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>114</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="H22" s="4"/>
       <c r="I22" s="4" t="s">
-        <v>36</v>
+        <v>238</v>
       </c>
       <c r="J22" t="s">
-        <v>36</v>
+        <v>238</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>201</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2201,16 +2218,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E23" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -2219,11 +2236,11 @@
         <v>21</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2231,16 +2248,16 @@
         <v>1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2252,10 +2269,10 @@
         <v>28</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2263,16 +2280,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2282,10 +2299,10 @@
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2293,16 +2310,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E26" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2312,10 +2329,10 @@
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2323,29 +2340,29 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E27" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2353,16 +2370,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E28" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -2372,10 +2389,10 @@
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -2383,110 +2400,110 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E29" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="K29" s="9" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E30" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>36</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="J31" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E32" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2501,24 +2518,24 @@
         <v>36</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="E33" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2533,33 +2550,33 @@
         <v>36</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>36</v>
@@ -2568,33 +2585,33 @@
         <v>36</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E35" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>36</v>
@@ -2603,24 +2620,24 @@
         <v>36</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E36" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2629,30 +2646,30 @@
         <v>22</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E37" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2661,27 +2678,27 @@
         <v>22</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="K37" s="9" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E38" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2690,56 +2707,56 @@
         <v>22</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="K38" s="9" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E39" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E40" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2748,56 +2765,56 @@
         <v>22</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E41" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E42" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -2812,30 +2829,30 @@
         <v>36</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E43" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>36</v>
@@ -2844,30 +2861,30 @@
         <v>36</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E44" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>36</v>
@@ -2876,30 +2893,30 @@
         <v>36</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E45" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>36</v>
@@ -2908,30 +2925,30 @@
         <v>36</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E46" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>36</v>
@@ -2940,24 +2957,24 @@
         <v>36</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E47" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2966,39 +2983,39 @@
         <v>21</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E48" t="s">
+        <v>234</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
         <v>96</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E48" t="s">
-        <v>240</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48" t="s">
-        <v>98</v>
-      </c>
       <c r="H48" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>36</v>
@@ -3007,24 +3024,24 @@
         <v>36</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>152</v>
+        <v>240</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>153</v>
+        <v>240</v>
       </c>
       <c r="E49" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -3033,27 +3050,27 @@
         <v>22</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E50" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -3062,17 +3079,49 @@
         <v>22</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K50" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="13" t="s">
         <v>239</v>
       </c>
+      <c r="C51" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51" t="s">
+        <v>242</v>
+      </c>
+      <c r="E51" t="s">
+        <v>234</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -3090,12 +3139,12 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moving the metadata into a table.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A13FE65-D63A-4B24-9DEE-30DCF465F34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494E414D-EE4D-4B69-B32D-00FA4192D0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42555" yWindow="1650" windowWidth="23355" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -963,10 +963,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1149,47 +1156,48 @@
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
@@ -1525,10 +1533,10 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2680,7 +2688,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="7" t="s">
         <v>228</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -3664,7 +3672,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="17" type="noConversion"/>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modularizing code base and addressing Stan's outstanding suggestions.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494E414D-EE4D-4B69-B32D-00FA4192D0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD12465-4B55-4068-909B-9C586A48EE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35160" yWindow="870" windowWidth="21705" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="309">
   <si>
     <t>Poultry</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Eggs Sold (Y/N)</t>
   </si>
   <si>
-    <t>Eggs Sold (Qty)</t>
-  </si>
-  <si>
     <t>Number of Chicken Eggs Sold</t>
   </si>
   <si>
@@ -758,9 +755,6 @@
     <t>Chicken Sale Price (head)</t>
   </si>
   <si>
-    <t>Chicken Sale Price (kg)</t>
-  </si>
-  <si>
     <t>Chicken Live Sale Price (KHR/kg, Average)</t>
   </si>
   <si>
@@ -957,16 +951,32 @@
   </si>
   <si>
     <t>animal_area</t>
+  </si>
+  <si>
+    <t>Chicken Sale Price</t>
+  </si>
+  <si>
+    <t>Eggs Sold</t>
+  </si>
+  <si>
+    <t>Chicken Morality Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1156,47 +1166,48 @@
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
@@ -1530,13 +1541,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I53" sqref="I53"/>
+      <selection pane="bottomRight" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,7 +1572,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1576,16 +1587,16 @@
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="L1" t="s">
         <v>33</v>
@@ -1598,10 +1609,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1619,21 +1630,21 @@
         <v>23</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -1656,19 +1667,19 @@
         <v>34</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -1691,7 +1702,7 @@
         <v>34</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M4" s="2"/>
     </row>
@@ -1700,10 +1711,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1721,10 +1732,10 @@
         <v>24</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1732,10 +1743,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1753,10 +1764,10 @@
         <v>25</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1764,10 +1775,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1782,16 +1793,16 @@
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J7" t="s">
         <v>26</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1799,10 +1810,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>241</v>
+        <v>306</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -1820,10 +1831,10 @@
         <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1834,7 +1845,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -1852,10 +1863,10 @@
         <v>28</v>
       </c>
       <c r="K9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1866,7 +1877,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -1881,16 +1892,16 @@
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J10" t="s">
         <v>29</v>
       </c>
       <c r="K10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1898,10 +1909,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1919,10 +1930,10 @@
         <v>30</v>
       </c>
       <c r="K11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1930,10 +1941,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -1951,10 +1962,10 @@
         <v>31</v>
       </c>
       <c r="K12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1965,7 +1976,7 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -1983,10 +1994,10 @@
         <v>32</v>
       </c>
       <c r="K13" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2012,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J14" t="s">
         <v>34</v>
@@ -2021,18 +2032,18 @@
         <v>34</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -2053,39 +2064,39 @@
         <v>34</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>94</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2093,10 +2104,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
+        <v>307</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
@@ -2117,7 +2128,7 @@
         <v>34</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2128,7 +2139,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -2137,13 +2148,13 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>34</v>
@@ -2152,7 +2163,7 @@
         <v>34</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2160,10 +2171,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
@@ -2172,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2184,50 +2195,50 @@
         <v>34</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>94</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
@@ -2236,10 +2247,10 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -2252,18 +2263,18 @@
         <v>34</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
@@ -2272,10 +2283,10 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
@@ -2288,18 +2299,18 @@
         <v>34</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
@@ -2308,10 +2319,10 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
@@ -2324,18 +2335,18 @@
         <v>34</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
@@ -2350,24 +2361,24 @@
         <v>0</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
@@ -2385,21 +2396,21 @@
         <v>26</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
         <v>0</v>
@@ -2414,25 +2425,25 @@
         <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
@@ -2447,25 +2458,25 @@
         <v>1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -2474,31 +2485,31 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
@@ -2513,25 +2524,25 @@
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
@@ -2540,64 +2551,64 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="D32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2605,7 +2616,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2617,19 +2628,19 @@
         <v>34</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="D33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2637,13 +2648,13 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>34</v>
@@ -2652,18 +2663,18 @@
         <v>34</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>0</v>
@@ -2672,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2684,85 +2695,85 @@
         <v>34</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K35" t="s">
+        <v>286</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>94</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="K36" t="s">
         <v>287</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>95</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="K36" t="s">
+      <c r="L36" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -2774,91 +2785,91 @@
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>34</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>34</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" t="s">
+        <v>304</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" t="s">
-        <v>306</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>97</v>
-      </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="D40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -2876,21 +2887,21 @@
         <v>34</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2908,30 +2919,30 @@
         <v>34</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
@@ -2944,30 +2955,30 @@
         <v>34</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
@@ -2980,21 +2991,21 @@
         <v>34</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -3006,27 +3017,27 @@
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -3038,27 +3049,27 @@
         <v>1</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -3070,59 +3081,59 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -3134,59 +3145,59 @@
         <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -3204,27 +3215,27 @@
         <v>34</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="D51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -3236,27 +3247,27 @@
         <v>34</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3268,33 +3279,33 @@
         <v>34</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>34</v>
@@ -3303,27 +3314,27 @@
         <v>34</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3335,21 +3346,21 @@
         <v>34</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -3361,36 +3372,36 @@
         <v>0</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
@@ -3403,21 +3414,21 @@
         <v>34</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -3429,27 +3440,27 @@
         <v>1</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -3461,27 +3472,27 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -3496,24 +3507,24 @@
         <v>25</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="D60" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -3525,62 +3536,62 @@
         <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="K61" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="L61" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="D62" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -3592,30 +3603,30 @@
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -3627,27 +3638,27 @@
         <v>0</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="D64" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -3659,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>34</v>
@@ -3668,11 +3679,37 @@
         <v>34</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sam's recent data update and new policy pathways table. Pushed to public.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD12465-4B55-4068-909B-9C586A48EE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6C60E2-7ABC-450E-A093-AA92A8B76ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35160" yWindow="870" windowWidth="21705" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="308">
   <si>
     <t>Poultry</t>
   </si>
@@ -957,26 +957,16 @@
   </si>
   <si>
     <t>Eggs Sold</t>
-  </si>
-  <si>
-    <t>Chicken Morality Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1166,48 +1156,47 @@
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
@@ -1541,13 +1530,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A68" sqref="A68"/>
+      <selection pane="bottomRight" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3682,34 +3671,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Visual improvements to the correlations tab and a few bugfixes.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6C60E2-7ABC-450E-A093-AA92A8B76ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33E1D84-CFE5-4056-9605-4C6F68795F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="311">
   <si>
     <t>Poultry</t>
   </si>
@@ -101,9 +101,6 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>currency/kg</t>
-  </si>
-  <si>
     <t>S4_Q14</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>ratio</t>
   </si>
   <si>
-    <t>currency</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
@@ -326,9 +320,6 @@
     <t>ha</t>
   </si>
   <si>
-    <t xml:space="preserve">currency </t>
-  </si>
-  <si>
     <t>Number of Chickens Owned (End of Survey Timeframe)</t>
   </si>
   <si>
@@ -761,9 +752,6 @@
     <t>Chicken Live Sale Price (KHR/head, Average)</t>
   </si>
   <si>
-    <t>currency/head</t>
-  </si>
-  <si>
     <t>Determined by multiplying "chicken sale price (KHR/kg)" by an average weight per bird</t>
   </si>
   <si>
@@ -957,6 +945,27 @@
   </si>
   <si>
     <t>Eggs Sold</t>
+  </si>
+  <si>
+    <t>hh_vars</t>
+  </si>
+  <si>
+    <t>KHR/kg</t>
+  </si>
+  <si>
+    <t>KHR</t>
+  </si>
+  <si>
+    <t>KHR/head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KHR </t>
+  </si>
+  <si>
+    <t>Chickens</t>
+  </si>
+  <si>
+    <t>Cattle</t>
   </si>
 </sst>
 </file>
@@ -1533,10 +1542,10 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G50" sqref="G50"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,10 +1567,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -1576,19 +1585,19 @@
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1598,10 +1607,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1610,30 +1619,30 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -1641,8 +1650,8 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
+      <c r="F3" t="s">
+        <v>309</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2">
@@ -1650,25 +1659,25 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -1676,8 +1685,8 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
+      <c r="F4" t="s">
+        <v>309</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2">
@@ -1685,13 +1694,13 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="M4" s="2"/>
     </row>
@@ -1700,10 +1709,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1712,19 +1721,19 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1732,10 +1741,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1744,19 +1753,19 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1764,10 +1773,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1776,22 +1785,22 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1799,10 +1808,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -1811,19 +1820,19 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>305</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1831,10 +1840,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -1843,19 +1852,19 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1863,10 +1872,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -1875,22 +1884,22 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1898,10 +1907,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1910,19 +1919,19 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1930,10 +1939,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -1942,19 +1951,19 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1962,10 +1971,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -1980,13 +1989,13 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1994,10 +2003,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
@@ -2006,33 +2015,33 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -2041,31 +2050,31 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>237</v>
-      </c>
       <c r="D16" s="2" t="s">
         <v>0</v>
       </c>
@@ -2073,19 +2082,19 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2093,10 +2102,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
@@ -2105,19 +2114,19 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2125,10 +2134,10 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -2137,22 +2146,22 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2160,10 +2169,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
@@ -2172,62 +2181,62 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>306</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
@@ -2236,34 +2245,34 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
@@ -2272,34 +2281,34 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
@@ -2308,34 +2317,34 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
@@ -2344,30 +2353,30 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
@@ -2382,24 +2391,24 @@
         <v>0</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
         <v>0</v>
@@ -2414,25 +2423,25 @@
         <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
@@ -2447,25 +2456,25 @@
         <v>1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -2474,31 +2483,31 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
@@ -2513,25 +2522,25 @@
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
@@ -2540,63 +2549,63 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>0</v>
@@ -2605,30 +2614,30 @@
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>242</v>
+        <v>307</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>0</v>
@@ -2637,132 +2646,132 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>92</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="K35" t="s">
         <v>282</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>94</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="K35" t="s">
-        <v>286</v>
-      </c>
       <c r="L35" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>92</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="K36" t="s">
+        <v>283</v>
+      </c>
+      <c r="L36" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>94</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="K36" t="s">
-        <v>287</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -2774,227 +2783,227 @@
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>20</v>
+        <v>310</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>20</v>
+        <v>310</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -3006,27 +3015,27 @@
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -3038,27 +3047,27 @@
         <v>1</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -3070,59 +3079,59 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -3134,59 +3143,59 @@
         <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -3198,226 +3207,226 @@
         <v>0</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>242</v>
+        <v>307</v>
       </c>
       <c r="H52">
         <v>0</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>97</v>
+        <v>308</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>97</v>
+        <v>308</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55" t="s">
-        <v>20</v>
+      <c r="F55" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -3429,27 +3438,27 @@
         <v>1</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -3461,27 +3470,27 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -3493,27 +3502,27 @@
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -3525,150 +3534,150 @@
         <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="D61" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E61">
         <v>1</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>242</v>
+        <v>307</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="J62" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H62">
-        <v>1</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="K62" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E63">
         <v>1</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>20</v>
+        <v>310</v>
       </c>
       <c r="H63">
         <v>0</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E64">
         <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>20</v>
+        <v>310</v>
       </c>
       <c r="H64">
         <v>1</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixes, accidentally created bug that's causing summary table to not filter.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33E1D84-CFE5-4056-9605-4C6F68795F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C69DE1-3446-467C-96CE-65B9456F4CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="312">
   <si>
     <t>Poultry</t>
   </si>
@@ -272,15 +272,9 @@
     <t>External Parasite Treatment (Y/N)</t>
   </si>
   <si>
-    <t>Chicken Vaccination Cost</t>
-  </si>
-  <si>
     <t>Chicken Medication Purchase (Y/N)</t>
   </si>
   <si>
-    <t>Cost of Medication for Chickens</t>
-  </si>
-  <si>
     <t>Rice Harvest (kg)</t>
   </si>
   <si>
@@ -290,15 +284,9 @@
     <t>Cattle Vaccination Rate</t>
   </si>
   <si>
-    <t>Cattle Vaccination Cost</t>
-  </si>
-  <si>
     <t>Cattle Medication Purchase (Y/N)</t>
   </si>
   <si>
-    <t>Cost of Cattle Medication</t>
-  </si>
-  <si>
     <t>Value of Cattle Produced</t>
   </si>
   <si>
@@ -413,18 +401,6 @@
     <t xml:space="preserve">Net Growth Rate </t>
   </si>
   <si>
-    <t>Chicken Vaccination Cost (KHR)</t>
-  </si>
-  <si>
-    <t>Cost of Medication for Chickens (KHR)</t>
-  </si>
-  <si>
-    <t>Cattle Vaccination Cost (KHR)</t>
-  </si>
-  <si>
-    <t>Cost of Cattle Medication (KHR)</t>
-  </si>
-  <si>
     <t>Unit Value of Slaughtered Cattle (KHR/head)</t>
   </si>
   <si>
@@ -966,6 +942,33 @@
   </si>
   <si>
     <t>Cattle</t>
+  </si>
+  <si>
+    <t>Chicken Vaccination Expenditure</t>
+  </si>
+  <si>
+    <t>Chicken Vaccination Expenditure (KHR)</t>
+  </si>
+  <si>
+    <t>Chicken Medication Expenditures</t>
+  </si>
+  <si>
+    <t>Chicken Medication Expenditures (KHR)</t>
+  </si>
+  <si>
+    <t>Cattle Vaccination Expenditures</t>
+  </si>
+  <si>
+    <t>Cattle Vaccination Expenditures (KHR)</t>
+  </si>
+  <si>
+    <t>Cattle Medication Expenditures</t>
+  </si>
+  <si>
+    <t>Cattle Medication Expenditures (KHR)</t>
+  </si>
+  <si>
+    <t>Eggs/Day</t>
   </si>
 </sst>
 </file>
@@ -1541,11 +1544,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,16 +1588,16 @@
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L1" t="s">
         <v>32</v>
@@ -1610,7 +1613,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1619,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1628,21 +1631,21 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -1651,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2">
@@ -1665,19 +1668,19 @@
         <v>33</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -1686,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2">
@@ -1700,7 +1703,7 @@
         <v>33</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="M4" s="2"/>
     </row>
@@ -1712,7 +1715,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1721,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1730,10 +1733,10 @@
         <v>23</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1744,7 +1747,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1753,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1762,10 +1765,10 @@
         <v>24</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1776,7 +1779,7 @@
         <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1785,22 +1788,22 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1808,10 +1811,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -1820,7 +1823,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1829,10 +1832,10 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1843,7 +1846,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -1852,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1861,10 +1864,10 @@
         <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1875,7 +1878,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -1884,22 +1887,22 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="J10" t="s">
         <v>28</v>
       </c>
       <c r="K10" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1907,10 +1910,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1919,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1928,10 +1931,10 @@
         <v>29</v>
       </c>
       <c r="K11" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1942,7 +1945,7 @@
         <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -1951,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1960,10 +1963,10 @@
         <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1992,10 +1995,10 @@
         <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2015,13 +2018,13 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J14" t="s">
         <v>33</v>
@@ -2030,18 +2033,18 @@
         <v>33</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -2050,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2062,18 +2065,18 @@
         <v>33</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>0</v>
@@ -2082,7 +2085,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2094,7 +2097,7 @@
         <v>33</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2102,7 +2105,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
@@ -2114,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2126,7 +2129,7 @@
         <v>33</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2146,13 +2149,13 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>33</v>
@@ -2161,7 +2164,7 @@
         <v>33</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2169,7 +2172,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>71</v>
@@ -2181,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2193,18 +2196,18 @@
         <v>33</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>0</v>
@@ -2213,7 +2216,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2225,12 +2228,12 @@
         <v>33</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>72</v>
@@ -2245,10 +2248,10 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -2261,12 +2264,12 @@
         <v>33</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B22" t="s">
         <v>73</v>
@@ -2281,10 +2284,10 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
@@ -2297,7 +2300,7 @@
         <v>33</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2308,7 +2311,7 @@
         <v>74</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
@@ -2317,10 +2320,10 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
@@ -2333,7 +2336,7 @@
         <v>33</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2353,19 +2356,19 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2394,10 +2397,10 @@
         <v>25</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2423,14 +2426,14 @@
         <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2456,14 +2459,14 @@
         <v>1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2471,10 +2474,10 @@
         <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>79</v>
+        <v>303</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>126</v>
+        <v>304</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -2483,31 +2486,31 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
@@ -2522,14 +2525,14 @@
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2537,10 +2540,10 @@
         <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>305</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>127</v>
+        <v>306</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
@@ -2549,31 +2552,31 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>0</v>
@@ -2582,7 +2585,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2594,18 +2597,18 @@
         <v>33</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>0</v>
@@ -2614,7 +2617,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2626,18 +2629,18 @@
         <v>33</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>0</v>
@@ -2646,13 +2649,13 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>33</v>
@@ -2661,27 +2664,27 @@
         <v>33</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2693,82 +2696,82 @@
         <v>33</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K35" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K36" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>50</v>
@@ -2783,13 +2786,13 @@
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2797,31 +2800,31 @@
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2829,42 +2832,42 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="C40" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D40" t="s">
         <v>50</v>
@@ -2873,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2885,18 +2888,18 @@
         <v>33</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
         <v>50</v>
@@ -2905,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2917,18 +2920,18 @@
         <v>33</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
         <v>50</v>
@@ -2937,10 +2940,10 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
@@ -2953,18 +2956,18 @@
         <v>33</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
         <v>50</v>
@@ -2973,10 +2976,10 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
@@ -2989,18 +2992,18 @@
         <v>33</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D44" t="s">
         <v>50</v>
@@ -3015,13 +3018,13 @@
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -3047,13 +3050,13 @@
         <v>1</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -3079,13 +3082,13 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3093,10 +3096,10 @@
         <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>307</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>128</v>
+        <v>308</v>
       </c>
       <c r="D47" t="s">
         <v>50</v>
@@ -3105,19 +3108,19 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3125,10 +3128,10 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -3143,13 +3146,13 @@
         <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -3157,10 +3160,10 @@
         <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>87</v>
+        <v>309</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>129</v>
+        <v>310</v>
       </c>
       <c r="D49" t="s">
         <v>50</v>
@@ -3169,30 +3172,30 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
         <v>50</v>
@@ -3213,7 +3216,7 @@
         <v>33</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3221,10 +3224,10 @@
         <v>58</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
         <v>50</v>
@@ -3233,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -3245,18 +3248,18 @@
         <v>33</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D52" t="s">
         <v>50</v>
@@ -3265,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3277,7 +3280,7 @@
         <v>33</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3285,10 +3288,10 @@
         <v>59</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D53" t="s">
         <v>50</v>
@@ -3297,13 +3300,13 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>33</v>
@@ -3312,7 +3315,7 @@
         <v>33</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3320,10 +3323,10 @@
         <v>60</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D54" t="s">
         <v>50</v>
@@ -3332,7 +3335,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3344,7 +3347,7 @@
         <v>33</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3352,10 +3355,10 @@
         <v>61</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D55" t="s">
         <v>50</v>
@@ -3364,19 +3367,19 @@
         <v>1</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3384,10 +3387,10 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D56" t="s">
         <v>50</v>
@@ -3396,10 +3399,10 @@
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
@@ -3412,18 +3415,18 @@
         <v>33</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D57" t="s">
         <v>50</v>
@@ -3438,24 +3441,24 @@
         <v>1</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D58" t="s">
         <v>50</v>
@@ -3470,24 +3473,24 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>50</v>
@@ -3505,21 +3508,21 @@
         <v>24</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>50</v>
@@ -3534,27 +3537,27 @@
         <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>50</v>
@@ -3563,30 +3566,30 @@
         <v>1</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>50</v>
@@ -3595,33 +3598,33 @@
         <v>1</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>50</v>
@@ -3630,30 +3633,30 @@
         <v>1</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H63">
         <v>0</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>50</v>
@@ -3662,13 +3665,13 @@
         <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H64">
         <v>1</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>33</v>
@@ -3677,7 +3680,7 @@
         <v>33</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bugs introduced by previous update; to do: province totals
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C69DE1-3446-467C-96CE-65B9456F4CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534396D9-EC57-48A5-9CC0-04FF3A1F2A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="313">
   <si>
     <t>Poultry</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Egg Price</t>
   </si>
   <si>
-    <t>Household Sold Eggs (Y/N)</t>
-  </si>
-  <si>
     <t>Chicken Egg Sale Revenue (KHR)</t>
   </si>
   <si>
@@ -554,9 +551,6 @@
     <t>Determined by multiplying "percentage of collected eggs that were sold" [questionnaire] by "Eggs per year"</t>
   </si>
   <si>
-    <t>Chicken Egg Price (KHR/egg)</t>
-  </si>
-  <si>
     <t>Determined by multiplying "eggs sold (qty)" by "egg price (KHR/egg)"</t>
   </si>
   <si>
@@ -969,6 +963,15 @@
   </si>
   <si>
     <t>Eggs/Day</t>
+  </si>
+  <si>
+    <t>KHR/Egg</t>
+  </si>
+  <si>
+    <t>Chicken Egg Price</t>
+  </si>
+  <si>
+    <t>Households Selling Eggs (Y/N)</t>
   </si>
 </sst>
 </file>
@@ -1545,10 +1548,10 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,16 +1591,16 @@
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="L1" t="s">
         <v>32</v>
@@ -1613,7 +1616,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1622,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1631,21 +1634,21 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -1654,7 +1657,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2">
@@ -1668,20 +1671,20 @@
         <v>33</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2">
@@ -1703,7 +1706,7 @@
         <v>33</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M4" s="2"/>
     </row>
@@ -1715,7 +1718,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -1724,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1733,10 +1736,10 @@
         <v>23</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1747,7 +1750,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -1756,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1765,10 +1768,10 @@
         <v>24</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1779,7 +1782,7 @@
         <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1788,22 +1791,22 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1811,10 +1814,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -1823,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1832,10 +1835,10 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1846,7 +1849,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -1855,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1864,10 +1867,10 @@
         <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1878,7 +1881,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -1887,22 +1890,22 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J10" t="s">
         <v>28</v>
       </c>
       <c r="K10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1910,10 +1913,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -1922,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1931,10 +1934,10 @@
         <v>29</v>
       </c>
       <c r="K11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1945,7 +1948,7 @@
         <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>173</v>
+        <v>311</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -1954,7 +1957,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1963,10 +1966,10 @@
         <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1977,7 +1980,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>312</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -1995,10 +1998,10 @@
         <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2018,13 +2021,13 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J14" t="s">
         <v>33</v>
@@ -2033,18 +2036,18 @@
         <v>33</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -2053,7 +2056,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2065,39 +2068,39 @@
         <v>33</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>296</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>298</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2105,7 +2108,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>42</v>
@@ -2117,7 +2120,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2129,7 +2132,7 @@
         <v>33</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2140,7 +2143,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -2149,13 +2152,13 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>33</v>
@@ -2164,7 +2167,7 @@
         <v>33</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2172,10 +2175,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
@@ -2184,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2196,50 +2199,50 @@
         <v>33</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>296</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>298</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
@@ -2248,10 +2251,10 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -2264,18 +2267,18 @@
         <v>33</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
@@ -2284,10 +2287,10 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
@@ -2300,7 +2303,7 @@
         <v>33</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2308,10 +2311,10 @@
         <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
@@ -2320,10 +2323,10 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
@@ -2336,7 +2339,7 @@
         <v>33</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2344,10 +2347,10 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
@@ -2356,19 +2359,19 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2376,10 +2379,10 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
@@ -2397,10 +2400,10 @@
         <v>25</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2408,10 +2411,10 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
         <v>0</v>
@@ -2426,14 +2429,14 @@
         <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2441,10 +2444,10 @@
         <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
@@ -2459,14 +2462,14 @@
         <v>1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2474,10 +2477,10 @@
         <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -2486,31 +2489,31 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
@@ -2525,14 +2528,14 @@
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2540,10 +2543,10 @@
         <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
@@ -2552,32 +2555,32 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="D31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2585,7 +2588,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2597,19 +2600,19 @@
         <v>33</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="D32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2617,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2629,19 +2632,19 @@
         <v>33</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="D33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2649,13 +2652,13 @@
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>33</v>
@@ -2664,27 +2667,27 @@
         <v>33</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2696,82 +2699,82 @@
         <v>33</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K35" t="s">
+        <v>272</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>87</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="K36" t="s">
         <v>273</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>88</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="K36" t="s">
+      <c r="L36" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>50</v>
@@ -2786,13 +2789,13 @@
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2800,31 +2803,31 @@
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2832,42 +2835,40 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s">
+        <v>290</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" t="s">
-        <v>292</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>90</v>
-      </c>
       <c r="H39">
         <v>1</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>290</v>
-      </c>
+      <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="D40" t="s">
         <v>50</v>
@@ -2876,7 +2877,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2888,18 +2889,18 @@
         <v>33</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D41" t="s">
         <v>50</v>
@@ -2908,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2920,18 +2921,18 @@
         <v>33</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
         <v>50</v>
@@ -2940,10 +2941,10 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
@@ -2956,18 +2957,18 @@
         <v>33</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
         <v>50</v>
@@ -2976,10 +2977,10 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
@@ -2992,18 +2993,18 @@
         <v>33</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D44" t="s">
         <v>50</v>
@@ -3018,13 +3019,13 @@
         <v>0</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -3032,10 +3033,10 @@
         <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
         <v>50</v>
@@ -3050,13 +3051,13 @@
         <v>1</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -3064,10 +3065,10 @@
         <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
         <v>50</v>
@@ -3082,13 +3083,13 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3096,10 +3097,10 @@
         <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D47" t="s">
         <v>50</v>
@@ -3108,19 +3109,19 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3128,10 +3129,10 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s">
         <v>50</v>
@@ -3146,13 +3147,13 @@
         <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -3160,10 +3161,10 @@
         <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D49" t="s">
         <v>50</v>
@@ -3172,30 +3173,30 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D50" t="s">
         <v>50</v>
@@ -3216,7 +3217,7 @@
         <v>33</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3224,10 +3225,10 @@
         <v>58</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="D51" t="s">
         <v>50</v>
@@ -3236,7 +3237,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -3248,18 +3249,18 @@
         <v>33</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
         <v>50</v>
@@ -3268,7 +3269,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3280,7 +3281,7 @@
         <v>33</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3288,10 +3289,10 @@
         <v>59</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D53" t="s">
         <v>50</v>
@@ -3300,13 +3301,13 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H53">
         <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>33</v>
@@ -3315,7 +3316,7 @@
         <v>33</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3323,10 +3324,10 @@
         <v>60</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D54" t="s">
         <v>50</v>
@@ -3335,7 +3336,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3347,7 +3348,7 @@
         <v>33</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -3355,10 +3356,10 @@
         <v>61</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D55" t="s">
         <v>50</v>
@@ -3367,19 +3368,19 @@
         <v>1</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -3387,10 +3388,10 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D56" t="s">
         <v>50</v>
@@ -3399,10 +3400,10 @@
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
@@ -3415,18 +3416,18 @@
         <v>33</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="D57" t="s">
         <v>50</v>
@@ -3441,24 +3442,24 @@
         <v>1</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D58" t="s">
         <v>50</v>
@@ -3473,24 +3474,24 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>50</v>
@@ -3508,21 +3509,21 @@
         <v>24</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>50</v>
@@ -3537,27 +3538,27 @@
         <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>50</v>
@@ -3566,30 +3567,30 @@
         <v>1</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>50</v>
@@ -3598,33 +3599,33 @@
         <v>1</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>50</v>
@@ -3633,30 +3634,30 @@
         <v>1</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H63">
         <v>0</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>50</v>
@@ -3665,13 +3666,13 @@
         <v>1</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H64">
         <v>1</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J64" s="2" t="s">
         <v>33</v>
@@ -3680,7 +3681,7 @@
         <v>33</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data, interface to BS v 5, added validation tab and zone map
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2B8672-916E-4AC7-9D48-EB4CBC8CBD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DA4A21-BEB7-41CD-9EAB-1FC8F09002C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="387">
   <si>
     <t>Poultry</t>
   </si>
@@ -422,9 +422,6 @@
     <t>Cattle Born</t>
   </si>
   <si>
-    <t>Cattle Used for Draugh (Y/N)</t>
-  </si>
-  <si>
     <t>Daily Egg Production</t>
   </si>
   <si>
@@ -1032,16 +1029,216 @@
   </si>
   <si>
     <t>Production Methods</t>
+  </si>
+  <si>
+    <t>Cattle Used for Draught</t>
+  </si>
+  <si>
+    <t>Household Raised Poultry</t>
+  </si>
+  <si>
+    <t>Households Raising Poultry (%)</t>
+  </si>
+  <si>
+    <t>Household Raised Cattle</t>
+  </si>
+  <si>
+    <t>Households Raising Cattle (%)</t>
+  </si>
+  <si>
+    <t>Household Raised Livestock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Households Raising Livestock (%) </t>
+  </si>
+  <si>
+    <t>fhh</t>
+  </si>
+  <si>
+    <t>Female-Headed Households</t>
+  </si>
+  <si>
+    <t>Female Headed Households (%)</t>
+  </si>
+  <si>
+    <t>ag_comm</t>
+  </si>
+  <si>
+    <t>Agricultural Community Memembership</t>
+  </si>
+  <si>
+    <t>ag_assoc</t>
+  </si>
+  <si>
+    <t>Agricultural Association Membership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household Membership in an Agricultural Community (%) </t>
+  </si>
+  <si>
+    <t>Household Membership in an Agricultural Association (%)</t>
+  </si>
+  <si>
+    <t>ag_extension</t>
+  </si>
+  <si>
+    <t>Households Receiving Extension Services</t>
+  </si>
+  <si>
+    <t>Households Receiving Extension Services (%)</t>
+  </si>
+  <si>
+    <t>raised_Poultry</t>
+  </si>
+  <si>
+    <t>raised_Cattle</t>
+  </si>
+  <si>
+    <t>raised_Livestock</t>
+  </si>
+  <si>
+    <t>raised_Buffalo</t>
+  </si>
+  <si>
+    <t>raised_Pigs</t>
+  </si>
+  <si>
+    <t>Households Raising Buffalo</t>
+  </si>
+  <si>
+    <t>Households Raising Pigs</t>
+  </si>
+  <si>
+    <t>Household Raising Buffalo (%)</t>
+  </si>
+  <si>
+    <t>Households Raising Pigs (%)</t>
+  </si>
+  <si>
+    <t>num_Pigs</t>
+  </si>
+  <si>
+    <t>num_Buffalo</t>
+  </si>
+  <si>
+    <t>live_sale_rate_Cattle</t>
+  </si>
+  <si>
+    <t>live_sale_rate_Pigs</t>
+  </si>
+  <si>
+    <t>live_sale_rate_Buffalo</t>
+  </si>
+  <si>
+    <t>sale_price_obs_Cattle</t>
+  </si>
+  <si>
+    <t>sale_price_obs_Buffalo</t>
+  </si>
+  <si>
+    <t>sale_price_obs_Pigs</t>
+  </si>
+  <si>
+    <t>prod_value_Buffalo</t>
+  </si>
+  <si>
+    <t>prod_value_Pigs</t>
+  </si>
+  <si>
+    <t>Number of Pigs Owned</t>
+  </si>
+  <si>
+    <t>Number of Buffalo Owned</t>
+  </si>
+  <si>
+    <t>Proportion of Cattle Herd Sold Live</t>
+  </si>
+  <si>
+    <t>Proportion of Pig Herd Sold Live</t>
+  </si>
+  <si>
+    <t>Proportion of Buffalo Herd Sold Live</t>
+  </si>
+  <si>
+    <t>Observed Sale Price for Cattle</t>
+  </si>
+  <si>
+    <t>Observed Sale Price for Buffalo</t>
+  </si>
+  <si>
+    <t>Observed Sale Price for Pigs</t>
+  </si>
+  <si>
+    <t>Total Value of Buffalo Produced</t>
+  </si>
+  <si>
+    <t>Total Value of Pigs Produced</t>
+  </si>
+  <si>
+    <t>Pigs</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>peak_num_Buffalo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peak_num_Pigs </t>
+  </si>
+  <si>
+    <t>vax_pct_Buffalo</t>
+  </si>
+  <si>
+    <t>vax_pct_Pigs</t>
+  </si>
+  <si>
+    <t>Vaccination Rate for Cattle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1238,47 +1435,52 @@
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1613,13 +1815,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C1" t="s">
         <v>37</v>
@@ -1663,10 +1865,10 @@
         <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>98</v>
@@ -1685,7 +1887,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>63</v>
@@ -1700,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1709,10 +1911,10 @@
         <v>22</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1720,7 +1922,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>92</v>
@@ -1735,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2">
@@ -1749,7 +1951,7 @@
         <v>33</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N3" s="2"/>
     </row>
@@ -1758,7 +1960,7 @@
         <v>97</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>93</v>
@@ -1773,7 +1975,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2">
@@ -1787,7 +1989,7 @@
         <v>33</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N4" s="2"/>
     </row>
@@ -1796,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
@@ -1811,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1820,10 +2022,10 @@
         <v>23</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1831,7 +2033,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s">
         <v>65</v>
@@ -1846,7 +2048,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1855,10 +2057,10 @@
         <v>24</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1866,7 +2068,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C7" t="s">
         <v>67</v>
@@ -1881,22 +2083,22 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K7" t="s">
         <v>25</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1904,13 +2106,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
@@ -1919,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1928,10 +2130,10 @@
         <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1939,7 +2141,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>34</v>
@@ -1954,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1963,10 +2165,10 @@
         <v>27</v>
       </c>
       <c r="L9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1974,7 +2176,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -1989,22 +2191,22 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K10" t="s">
         <v>28</v>
       </c>
       <c r="L10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2012,10 +2214,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>116</v>
@@ -2027,7 +2229,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2036,10 +2238,10 @@
         <v>29</v>
       </c>
       <c r="L11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2047,13 +2249,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C12" t="s">
         <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
@@ -2062,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -2071,10 +2273,10 @@
         <v>30</v>
       </c>
       <c r="L12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2082,13 +2284,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
@@ -2106,10 +2308,10 @@
         <v>31</v>
       </c>
       <c r="L13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2117,7 +2319,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -2132,13 +2334,13 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K14" t="s">
         <v>33</v>
@@ -2147,7 +2349,7 @@
         <v>33</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2155,7 +2357,7 @@
         <v>117</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
@@ -2170,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -2182,42 +2384,42 @@
         <v>33</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>294</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>295</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2225,10 +2427,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>42</v>
@@ -2240,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2252,7 +2454,7 @@
         <v>33</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2260,7 +2462,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -2275,13 +2477,13 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>33</v>
@@ -2290,7 +2492,7 @@
         <v>33</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2298,7 +2500,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>119</v>
@@ -2313,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2325,50 +2527,50 @@
         <v>33</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>294</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>295</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>71</v>
@@ -2399,15 +2601,15 @@
         <v>33</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C22" t="s">
         <v>72</v>
@@ -2438,7 +2640,7 @@
         <v>33</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2446,7 +2648,7 @@
         <v>43</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>73</v>
@@ -2477,7 +2679,7 @@
         <v>33</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2485,7 +2687,7 @@
         <v>44</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C24" t="s">
         <v>74</v>
@@ -2500,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I24" s="2">
         <v>0</v>
@@ -2512,7 +2714,7 @@
         <v>33</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2520,13 +2722,13 @@
         <v>45</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C25" t="s">
         <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E25" t="s">
         <v>0</v>
@@ -2544,10 +2746,10 @@
         <v>25</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2555,13 +2757,13 @@
         <v>46</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C26" t="s">
         <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E26" t="s">
         <v>0</v>
@@ -2576,14 +2778,14 @@
         <v>1</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2591,13 +2793,13 @@
         <v>47</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C27" t="s">
         <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E27" t="s">
         <v>0</v>
@@ -2612,14 +2814,14 @@
         <v>1</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2627,14 +2829,14 @@
         <v>48</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="E28" t="s">
         <v>0</v>
       </c>
@@ -2642,34 +2844,34 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I28">
         <v>1</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C29" t="s">
         <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E29" t="s">
         <v>0</v>
@@ -2684,14 +2886,14 @@
         <v>1</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2699,14 +2901,14 @@
         <v>49</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C30" t="s">
+        <v>301</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>303</v>
-      </c>
       <c r="E30" t="s">
         <v>0</v>
       </c>
@@ -2714,69 +2916,69 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I30">
         <v>1</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M31" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>0</v>
@@ -2785,7 +2987,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -2797,62 +2999,62 @@
         <v>33</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M33" s="4" t="s">
         <v>233</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2870,24 +3072,24 @@
         <v>33</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2899,30 +3101,30 @@
         <v>1</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L35" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="E36" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2934,27 +3136,27 @@
         <v>1</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L36" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>50</v>
@@ -2975,7 +3177,7 @@
         <v>33</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2983,7 +3185,7 @@
         <v>51</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C38" t="s">
         <v>79</v>
@@ -2992,7 +3194,7 @@
         <v>79</v>
       </c>
       <c r="E38" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -3004,13 +3206,13 @@
         <v>0</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>33</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -3018,7 +3220,7 @@
         <v>52</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C39" t="s">
         <v>88</v>
@@ -3027,7 +3229,7 @@
         <v>88</v>
       </c>
       <c r="E39" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -3040,10 +3242,10 @@
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -3051,7 +3253,7 @@
         <v>100</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>104</v>
@@ -3066,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -3078,7 +3280,7 @@
         <v>33</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3086,7 +3288,7 @@
         <v>101</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>102</v>
@@ -3101,7 +3303,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -3113,15 +3315,15 @@
         <v>33</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>80</v>
@@ -3152,15 +3354,15 @@
         <v>33</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C43" t="s">
         <v>81</v>
@@ -3191,21 +3393,21 @@
         <v>33</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>110</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E44" t="s">
         <v>50</v>
@@ -3220,13 +3422,13 @@
         <v>0</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -3234,13 +3436,13 @@
         <v>53</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C45" t="s">
         <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E45" t="s">
         <v>50</v>
@@ -3255,13 +3457,13 @@
         <v>1</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -3269,13 +3471,13 @@
         <v>54</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C46" t="s">
         <v>77</v>
       </c>
       <c r="D46" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E46" t="s">
         <v>50</v>
@@ -3290,13 +3492,13 @@
         <v>1</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L46" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -3304,13 +3506,13 @@
         <v>55</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C47" t="s">
+        <v>303</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="E47" t="s">
         <v>50</v>
@@ -3319,19 +3521,19 @@
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I47">
         <v>1</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L47" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -3339,13 +3541,13 @@
         <v>56</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E48" t="s">
         <v>50</v>
@@ -3360,13 +3562,13 @@
         <v>1</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -3374,13 +3576,13 @@
         <v>57</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C49" t="s">
+        <v>305</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="E49" t="s">
         <v>50</v>
@@ -3389,27 +3591,27 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I49">
         <v>1</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L49" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>107</v>
@@ -3436,7 +3638,7 @@
         <v>33</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -3444,7 +3646,7 @@
         <v>58</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>122</v>
@@ -3459,7 +3661,7 @@
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -3471,7 +3673,7 @@
         <v>33</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3479,7 +3681,7 @@
         <v>109</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>124</v>
@@ -3494,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -3506,7 +3708,7 @@
         <v>33</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3514,7 +3716,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>83</v>
@@ -3529,13 +3731,13 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I53">
         <v>1</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>33</v>
@@ -3544,7 +3746,7 @@
         <v>33</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3552,10 +3754,10 @@
         <v>60</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>126</v>
@@ -3567,7 +3769,7 @@
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -3579,7 +3781,7 @@
         <v>33</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3587,7 +3789,7 @@
         <v>61</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>128</v>
@@ -3602,19 +3804,19 @@
         <v>1</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I55">
         <v>0</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3622,7 +3824,7 @@
         <v>62</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C56" t="s">
         <v>84</v>
@@ -3653,21 +3855,21 @@
         <v>33</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B57" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="D57" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E57" t="s">
         <v>50</v>
@@ -3682,27 +3884,27 @@
         <v>1</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C58" t="s">
         <v>85</v>
       </c>
       <c r="D58" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E58" t="s">
         <v>50</v>
@@ -3717,27 +3919,27 @@
         <v>0</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B59" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>50</v>
@@ -3755,24 +3957,24 @@
         <v>24</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>50</v>
@@ -3787,30 +3989,30 @@
         <v>1</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>50</v>
@@ -3819,33 +4021,33 @@
         <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I61">
         <v>0</v>
       </c>
       <c r="K61" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="L61" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="L61" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="M61" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B62" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>50</v>
@@ -3854,36 +4056,36 @@
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I62">
         <v>1</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>50</v>
@@ -3892,33 +4094,33 @@
         <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I63">
         <v>0</v>
       </c>
       <c r="K63" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="L63" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="L63" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="M63" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>50</v>
@@ -3927,13 +4129,13 @@
         <v>1</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I64">
         <v>1</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>33</v>
@@ -3942,21 +4144,21 @@
         <v>33</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C65" t="s">
         <v>320</v>
       </c>
-      <c r="B65" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C65" t="s">
-        <v>321</v>
-      </c>
       <c r="D65" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>0</v>
@@ -3965,7 +4167,7 @@
         <v>0</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2">
@@ -3976,8 +4178,578 @@
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
     </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C66" t="s">
+        <v>333</v>
+      </c>
+      <c r="D66" t="s">
+        <v>334</v>
+      </c>
+      <c r="E66" t="s">
+        <v>292</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66" t="s">
+        <v>21</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C67" t="s">
+        <v>335</v>
+      </c>
+      <c r="D67" t="s">
+        <v>336</v>
+      </c>
+      <c r="E67" t="s">
+        <v>50</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67" t="s">
+        <v>21</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C68" t="s">
+        <v>337</v>
+      </c>
+      <c r="D68" t="s">
+        <v>338</v>
+      </c>
+      <c r="E68" t="s">
+        <v>292</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68" t="s">
+        <v>21</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C69" t="s">
+        <v>340</v>
+      </c>
+      <c r="D69" t="s">
+        <v>341</v>
+      </c>
+      <c r="E69" t="s">
+        <v>292</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69" t="s">
+        <v>21</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C70" t="s">
+        <v>343</v>
+      </c>
+      <c r="D70" t="s">
+        <v>346</v>
+      </c>
+      <c r="E70" t="s">
+        <v>292</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" t="s">
+        <v>21</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C71" t="s">
+        <v>345</v>
+      </c>
+      <c r="D71" t="s">
+        <v>347</v>
+      </c>
+      <c r="E71" t="s">
+        <v>292</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71" t="s">
+        <v>21</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C72" t="s">
+        <v>349</v>
+      </c>
+      <c r="D72" t="s">
+        <v>350</v>
+      </c>
+      <c r="E72" t="s">
+        <v>292</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72" t="s">
+        <v>21</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="C73" t="s">
+        <v>356</v>
+      </c>
+      <c r="D73" t="s">
+        <v>358</v>
+      </c>
+      <c r="E73" t="s">
+        <v>50</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73" t="s">
+        <v>21</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="C74" t="s">
+        <v>357</v>
+      </c>
+      <c r="D74" t="s">
+        <v>359</v>
+      </c>
+      <c r="E74" t="s">
+        <v>50</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74" t="s">
+        <v>21</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C75" t="s">
+        <v>370</v>
+      </c>
+      <c r="D75" t="s">
+        <v>370</v>
+      </c>
+      <c r="E75" t="s">
+        <v>50</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75" t="s">
+        <v>380</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C76" t="s">
+        <v>371</v>
+      </c>
+      <c r="D76" t="s">
+        <v>371</v>
+      </c>
+      <c r="E76" t="s">
+        <v>50</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76" t="s">
+        <v>381</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C77" t="s">
+        <v>372</v>
+      </c>
+      <c r="D77" t="s">
+        <v>372</v>
+      </c>
+      <c r="E77" t="s">
+        <v>50</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77" t="s">
+        <v>86</v>
+      </c>
+      <c r="H77" t="s">
+        <v>101</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C78" t="s">
+        <v>373</v>
+      </c>
+      <c r="D78" t="s">
+        <v>373</v>
+      </c>
+      <c r="E78" t="s">
+        <v>50</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78" t="s">
+        <v>86</v>
+      </c>
+      <c r="H78" t="s">
+        <v>383</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C79" t="s">
+        <v>374</v>
+      </c>
+      <c r="D79" t="s">
+        <v>374</v>
+      </c>
+      <c r="E79" t="s">
+        <v>50</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79" t="s">
+        <v>86</v>
+      </c>
+      <c r="H79" t="s">
+        <v>382</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C80" t="s">
+        <v>375</v>
+      </c>
+      <c r="D80" t="s">
+        <v>375</v>
+      </c>
+      <c r="E80" t="s">
+        <v>50</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80" t="s">
+        <v>295</v>
+      </c>
+      <c r="H80" t="s">
+        <v>101</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C81" t="s">
+        <v>376</v>
+      </c>
+      <c r="D81" t="s">
+        <v>376</v>
+      </c>
+      <c r="E81" t="s">
+        <v>50</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81" t="s">
+        <v>295</v>
+      </c>
+      <c r="H81" t="s">
+        <v>383</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C82" t="s">
+        <v>377</v>
+      </c>
+      <c r="D82" t="s">
+        <v>377</v>
+      </c>
+      <c r="E82" t="s">
+        <v>50</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82" t="s">
+        <v>295</v>
+      </c>
+      <c r="H82" t="s">
+        <v>382</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C83" t="s">
+        <v>378</v>
+      </c>
+      <c r="D83" t="s">
+        <v>378</v>
+      </c>
+      <c r="E83" t="s">
+        <v>50</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="G83" t="s">
+        <v>294</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C84" t="s">
+        <v>379</v>
+      </c>
+      <c r="D84" t="s">
+        <v>379</v>
+      </c>
+      <c r="E84" t="s">
+        <v>50</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84" t="s">
+        <v>294</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="C85" t="s">
+        <v>386</v>
+      </c>
+      <c r="D85" t="s">
+        <v>386</v>
+      </c>
+      <c r="E85" t="s">
+        <v>50</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85" t="s">
+        <v>86</v>
+      </c>
+      <c r="H85" t="s">
+        <v>382</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="C86" t="s">
+        <v>386</v>
+      </c>
+      <c r="D86" t="s">
+        <v>386</v>
+      </c>
+      <c r="E86" t="s">
+        <v>50</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86" t="s">
+        <v>86</v>
+      </c>
+      <c r="H86" t="s">
+        <v>383</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished updates, final build before presentation
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DA4A21-BEB7-41CD-9EAB-1FC8F09002C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D878861B-4169-4B7C-A82F-280566164CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1121,15 +1121,6 @@
     <t>num_Buffalo</t>
   </si>
   <si>
-    <t>live_sale_rate_Cattle</t>
-  </si>
-  <si>
-    <t>live_sale_rate_Pigs</t>
-  </si>
-  <si>
-    <t>live_sale_rate_Buffalo</t>
-  </si>
-  <si>
     <t>sale_price_obs_Cattle</t>
   </si>
   <si>
@@ -1194,16 +1185,32 @@
   </si>
   <si>
     <t>Vaccination Rate for Cattle</t>
+  </si>
+  <si>
+    <t>sale_rate_Buffalo</t>
+  </si>
+  <si>
+    <t>sale_rate_Pigs</t>
+  </si>
+  <si>
+    <t>sale_rate_Cattle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1435,47 +1442,48 @@
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1818,10 +1826,10 @@
   <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I87" sqref="I87"/>
+      <selection pane="bottomRight" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3623,7 +3631,7 @@
         <v>50</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" t="s">
         <v>20</v>
@@ -4420,19 +4428,19 @@
         <v>318</v>
       </c>
       <c r="C75" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D75" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E75" t="s">
         <v>50</v>
       </c>
       <c r="F75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -4446,36 +4454,36 @@
         <v>318</v>
       </c>
       <c r="C76" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D76" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E76" t="s">
         <v>50</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I76">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
-        <v>362</v>
+      <c r="A77" s="14" t="s">
+        <v>386</v>
       </c>
       <c r="B77" s="12" t="s">
         <v>313</v>
       </c>
       <c r="C77" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D77" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E77" t="s">
         <v>50</v>
@@ -4494,17 +4502,17 @@
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>363</v>
+      <c r="A78" s="14" t="s">
+        <v>385</v>
       </c>
       <c r="B78" s="12" t="s">
         <v>313</v>
       </c>
       <c r="C78" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D78" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E78" t="s">
         <v>50</v>
@@ -4516,24 +4524,24 @@
         <v>86</v>
       </c>
       <c r="H78" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="I78">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>364</v>
+      <c r="A79" s="14" t="s">
+        <v>384</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>313</v>
       </c>
       <c r="C79" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D79" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E79" t="s">
         <v>50</v>
@@ -4545,7 +4553,7 @@
         <v>86</v>
       </c>
       <c r="H79" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I79">
         <v>0</v>
@@ -4553,16 +4561,16 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>313</v>
       </c>
       <c r="C80" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D80" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E80" t="s">
         <v>50</v>
@@ -4582,16 +4590,16 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B81" s="12" t="s">
         <v>313</v>
       </c>
       <c r="C81" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D81" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E81" t="s">
         <v>50</v>
@@ -4603,7 +4611,7 @@
         <v>295</v>
       </c>
       <c r="H81" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="I81">
         <v>0</v>
@@ -4611,16 +4619,16 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B82" s="12" t="s">
         <v>313</v>
       </c>
       <c r="C82" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D82" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E82" t="s">
         <v>50</v>
@@ -4632,7 +4640,7 @@
         <v>295</v>
       </c>
       <c r="H82" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I82">
         <v>0</v>
@@ -4640,16 +4648,16 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B83" s="12" t="s">
         <v>313</v>
       </c>
       <c r="C83" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D83" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E83" t="s">
         <v>50</v>
@@ -4666,16 +4674,16 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>313</v>
       </c>
       <c r="C84" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D84" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E84" t="s">
         <v>50</v>
@@ -4692,16 +4700,16 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>315</v>
       </c>
       <c r="C85" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D85" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E85" t="s">
         <v>50</v>
@@ -4713,7 +4721,7 @@
         <v>86</v>
       </c>
       <c r="H85" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I85">
         <v>0</v>
@@ -4721,16 +4729,16 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>315</v>
       </c>
       <c r="C86" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D86" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E86" t="s">
         <v>50</v>
@@ -4742,14 +4750,14 @@
         <v>86</v>
       </c>
       <c r="H86" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="I86">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="24" type="noConversion"/>
+  <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last several weeks of updates and edits.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D878861B-4169-4B7C-A82F-280566164CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472AA083-23FE-4301-A040-9FD03647F379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="422">
   <si>
     <t>Poultry</t>
   </si>
@@ -1194,16 +1194,128 @@
   </si>
   <si>
     <t>sale_rate_Cattle</t>
+  </si>
+  <si>
+    <t>cashew</t>
+  </si>
+  <si>
+    <t>area_cashew_harvested</t>
+  </si>
+  <si>
+    <t>area_cashew_planted</t>
+  </si>
+  <si>
+    <t>qty_cashew_own_use</t>
+  </si>
+  <si>
+    <t>qty_cashew_sale</t>
+  </si>
+  <si>
+    <t>qty_cashew_gift</t>
+  </si>
+  <si>
+    <t>qty_cashew_pay</t>
+  </si>
+  <si>
+    <t>qty_cashew_feed</t>
+  </si>
+  <si>
+    <t>qty_cashew_seed</t>
+  </si>
+  <si>
+    <t>qty_cashew_lost</t>
+  </si>
+  <si>
+    <t>qty_cashew_processed</t>
+  </si>
+  <si>
+    <t>Households Cultivating Cashews</t>
+  </si>
+  <si>
+    <t>Percent of Households Cultivating Cashews</t>
+  </si>
+  <si>
+    <t>Area of Cashews Harvested</t>
+  </si>
+  <si>
+    <t>Area of Cashews Planted</t>
+  </si>
+  <si>
+    <t>Area of Cashews Harvested (ha)</t>
+  </si>
+  <si>
+    <t>Ha</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Kept</t>
+  </si>
+  <si>
+    <t>Area of Cashews Planted (ha)</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Kept (kg)</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Sold</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Sold (kg)</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Gifted</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Given as Gifts (kg)</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Given as Payments</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Used for Animal Feed</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Used for Seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity of Cashews Lost </t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Damaged</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Given as Payment (kg)</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Used for Animal Feed (kg)</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Lost (kg)</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Damaged (kg)</t>
+  </si>
+  <si>
+    <t>Quantity of Cashews Used for Seed (kg)</t>
+  </si>
+  <si>
+    <t>Kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1442,47 +1554,48 @@
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1823,13 +1936,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O86"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F80" sqref="F80"/>
+      <selection pane="bottomRight" activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4756,8 +4869,294 @@
         <v>0</v>
       </c>
     </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C87" t="s">
+        <v>398</v>
+      </c>
+      <c r="D87" t="s">
+        <v>399</v>
+      </c>
+      <c r="E87" t="s">
+        <v>288</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>21</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C88" t="s">
+        <v>400</v>
+      </c>
+      <c r="D88" t="s">
+        <v>402</v>
+      </c>
+      <c r="E88" t="s">
+        <v>288</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88" t="s">
+        <v>403</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C89" t="s">
+        <v>401</v>
+      </c>
+      <c r="D89" t="s">
+        <v>405</v>
+      </c>
+      <c r="E89" t="s">
+        <v>288</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89" t="s">
+        <v>403</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C90" t="s">
+        <v>404</v>
+      </c>
+      <c r="D90" t="s">
+        <v>406</v>
+      </c>
+      <c r="E90" t="s">
+        <v>288</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90" t="s">
+        <v>403</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C91" t="s">
+        <v>407</v>
+      </c>
+      <c r="D91" t="s">
+        <v>408</v>
+      </c>
+      <c r="E91" t="s">
+        <v>288</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91" t="s">
+        <v>421</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C92" t="s">
+        <v>409</v>
+      </c>
+      <c r="D92" t="s">
+        <v>410</v>
+      </c>
+      <c r="E92" t="s">
+        <v>288</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92" t="s">
+        <v>421</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C93" t="s">
+        <v>411</v>
+      </c>
+      <c r="D93" t="s">
+        <v>416</v>
+      </c>
+      <c r="E93" t="s">
+        <v>288</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93" t="s">
+        <v>421</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C94" t="s">
+        <v>412</v>
+      </c>
+      <c r="D94" t="s">
+        <v>417</v>
+      </c>
+      <c r="E94" t="s">
+        <v>288</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94" t="s">
+        <v>421</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C95" t="s">
+        <v>413</v>
+      </c>
+      <c r="D95" t="s">
+        <v>420</v>
+      </c>
+      <c r="E95" t="s">
+        <v>288</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95" t="s">
+        <v>421</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C96" t="s">
+        <v>414</v>
+      </c>
+      <c r="D96" t="s">
+        <v>418</v>
+      </c>
+      <c r="E96" t="s">
+        <v>288</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96" t="s">
+        <v>421</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="15" t="s">
+        <v>397</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C97" t="s">
+        <v>415</v>
+      </c>
+      <c r="D97" t="s">
+        <v>419</v>
+      </c>
+      <c r="E97" t="s">
+        <v>288</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97" t="s">
+        <v>421</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="25" type="noConversion"/>
+  <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* Removed archived data/update files * Minor functionality changes in startup (instrument_list is no longer necessary but kept in just in case) * Update old renv.lock * Efficiency edits * Added example translation of landing page (change from en to km on line 84 of app.R to see the difference) * Minor bugfixes related to data input and processing
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472AA083-23FE-4301-A040-9FD03647F379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7100BF5-6645-4DF7-B9F3-52824DE97568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="424">
   <si>
     <t>Poultry</t>
   </si>
@@ -1299,6 +1299,12 @@
   </si>
   <si>
     <t>Kg</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>Only 258 households reported purchasing chickens in 2022</t>
   </si>
 </sst>
 </file>
@@ -1939,10 +1945,10 @@
   <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>297</v>
+        <v>422</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -2563,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>297</v>
+        <v>422</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2826,7 +2832,10 @@
         <v>297</v>
       </c>
       <c r="I24" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>423</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
Update old renv.lock, efficiency edits, added example translation of landing page, continuing to clean out old files.
</commit_message>
<xml_diff>
--- a/agquery/Update/indicators.xlsx
+++ b/agquery/Update/indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472AA083-23FE-4301-A040-9FD03647F379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7100BF5-6645-4DF7-B9F3-52824DE97568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="424">
   <si>
     <t>Poultry</t>
   </si>
@@ -1299,6 +1299,12 @@
   </si>
   <si>
     <t>Kg</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>Only 258 households reported purchasing chickens in 2022</t>
   </si>
 </sst>
 </file>
@@ -1939,10 +1945,10 @@
   <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>297</v>
+        <v>422</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -2563,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>297</v>
+        <v>422</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2826,7 +2832,10 @@
         <v>297</v>
       </c>
       <c r="I24" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>423</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>95</v>

</xml_diff>